<commit_message>
added 230 packet run MW 1D
</commit_message>
<xml_diff>
--- a/50TrialsVaryPackets.xlsx
+++ b/50TrialsVaryPackets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\AP-Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE71D59C-8C66-40EA-AE64-D27E4A4964B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804E305C-E450-4D70-A88A-23844BAB8B25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="12">
   <si>
     <t>Acc</t>
   </si>
@@ -7478,15 +7478,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A06EE43-A370-47E6-9A9B-D644A56FBF0A}">
-  <dimension ref="A1:S51"/>
+  <dimension ref="A1:W51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T12" sqref="T12"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
@@ -7502,8 +7502,11 @@
       <c r="R1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -7549,8 +7552,17 @@
       <c r="S2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>89.899682998657198</v>
       </c>
@@ -7587,8 +7599,17 @@
       <c r="O3">
         <v>551.36055135726895</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q3">
+        <v>87.703657150268498</v>
+      </c>
+      <c r="R3">
+        <v>0.32339541383366199</v>
+      </c>
+      <c r="S3">
+        <v>513.13632917404095</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>89.669644832610999</v>
       </c>
@@ -7625,8 +7646,17 @@
       <c r="O4">
         <v>544.04951500892605</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q4">
+        <v>89.245146512985201</v>
+      </c>
+      <c r="R4">
+        <v>0.254406929885792</v>
+      </c>
+      <c r="S4">
+        <v>502.66289806365899</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>87.739229202270494</v>
       </c>
@@ -7663,8 +7693,17 @@
       <c r="O5">
         <v>542.28713583946205</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q5">
+        <v>89.223802089691105</v>
+      </c>
+      <c r="R5">
+        <v>0.259136820126531</v>
+      </c>
+      <c r="S5">
+        <v>501.67518973350502</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>87.928950786590505</v>
       </c>
@@ -7701,8 +7740,17 @@
       <c r="O6">
         <v>546.41168141364994</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q6">
+        <v>88.185071945190401</v>
+      </c>
+      <c r="R6">
+        <v>0.27531552605310899</v>
+      </c>
+      <c r="S6">
+        <v>498.93015694618202</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>87.656223773956299</v>
       </c>
@@ -7739,8 +7787,17 @@
       <c r="O7">
         <v>541.61022663116398</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q7">
+        <v>89.026963710784898</v>
+      </c>
+      <c r="R7">
+        <v>0.249530878661437</v>
+      </c>
+      <c r="S7">
+        <v>499.93049550056401</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>89.000874757766695</v>
       </c>
@@ -7777,8 +7834,17 @@
       <c r="O8">
         <v>542.92116403579701</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q8">
+        <v>89.589017629623399</v>
+      </c>
+      <c r="R8">
+        <v>0.273849304244485</v>
+      </c>
+      <c r="S8">
+        <v>502.08425998687699</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>89.169257879257202</v>
       </c>
@@ -7815,8 +7881,17 @@
       <c r="O9">
         <v>545.85422968864395</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q9">
+        <v>89.854627847671495</v>
+      </c>
+      <c r="R9">
+        <v>0.23938763019855799</v>
+      </c>
+      <c r="S9">
+        <v>501.63039469718899</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>89.216685295104895</v>
       </c>
@@ -7853,8 +7928,17 @@
       <c r="O10">
         <v>547.05730724334705</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q10">
+        <v>87.841200828552203</v>
+      </c>
+      <c r="R10">
+        <v>0.28207105664682902</v>
+      </c>
+      <c r="S10">
+        <v>499.93942928314198</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>89.356607198715196</v>
       </c>
@@ -7891,8 +7975,17 @@
       <c r="O11">
         <v>544.99331116676296</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q11">
+        <v>88.208788633346501</v>
+      </c>
+      <c r="R11">
+        <v>0.29210190150156001</v>
+      </c>
+      <c r="S11">
+        <v>504.15216732025101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>88.744753599166799</v>
       </c>
@@ -7929,8 +8022,17 @@
       <c r="O12">
         <v>546.16639089584305</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q12">
+        <v>88.374793529510498</v>
+      </c>
+      <c r="R12">
+        <v>0.25190459219327799</v>
+      </c>
+      <c r="S12">
+        <v>502.88548517227099</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>88.946330547332707</v>
       </c>
@@ -7967,8 +8069,17 @@
       <c r="O13">
         <v>546.45408487319901</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q13">
+        <v>89.603245258331299</v>
+      </c>
+      <c r="R13">
+        <v>0.280288274066054</v>
+      </c>
+      <c r="S13">
+        <v>503.613765001297</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>88.317877054214406</v>
       </c>
@@ -8005,8 +8116,17 @@
       <c r="O14">
         <v>546.16273212432804</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q14">
+        <v>89.152652025222693</v>
+      </c>
+      <c r="R14">
+        <v>0.25122237992315799</v>
+      </c>
+      <c r="S14">
+        <v>503.34356117248501</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>89.446723461151095</v>
       </c>
@@ -8043,8 +8163,17 @@
       <c r="O15">
         <v>546.87314581870999</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q15">
+        <v>88.955819606781006</v>
+      </c>
+      <c r="R15">
+        <v>0.262904541021033</v>
+      </c>
+      <c r="S15">
+        <v>501.38673090934702</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>88.227760791778493</v>
       </c>
@@ -8081,8 +8210,17 @@
       <c r="O16">
         <v>547.32949757575898</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q16">
+        <v>89.155024290084796</v>
+      </c>
+      <c r="R16">
+        <v>0.25923464412610497</v>
+      </c>
+      <c r="S16">
+        <v>503.03025245666498</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>89.000874757766695</v>
       </c>
@@ -8119,8 +8257,17 @@
       <c r="O17">
         <v>545.30119872093201</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q17">
+        <v>88.346338272094698</v>
+      </c>
+      <c r="R17">
+        <v>0.26661843286817999</v>
+      </c>
+      <c r="S17">
+        <v>502.25094246864302</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>89.211940765380803</v>
       </c>
@@ -8157,8 +8304,17 @@
       <c r="O18">
         <v>545.76163697242703</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q18">
+        <v>89.173996448516803</v>
+      </c>
+      <c r="R18">
+        <v>0.25083581785206399</v>
+      </c>
+      <c r="S18">
+        <v>503.68373632431002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>88.251477479934593</v>
       </c>
@@ -8195,8 +8351,17 @@
       <c r="O19">
         <v>545.28115653991699</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q19">
+        <v>88.789814710616994</v>
+      </c>
+      <c r="R19">
+        <v>0.263333906400956</v>
+      </c>
+      <c r="S19">
+        <v>502.88818001747097</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>88.075983524322496</v>
       </c>
@@ -8233,8 +8398,17 @@
       <c r="O20">
         <v>545.80812358856201</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q20">
+        <v>87.5803351402282</v>
+      </c>
+      <c r="R20">
+        <v>0.32525435395212399</v>
+      </c>
+      <c r="S20">
+        <v>499.70321536064102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>88.993763923645005</v>
       </c>
@@ -8271,8 +8445,17 @@
       <c r="O21">
         <v>547.65209531784001</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q21">
+        <v>88.853842020034705</v>
+      </c>
+      <c r="R21">
+        <v>0.28285851866833001</v>
+      </c>
+      <c r="S21">
+        <v>503.92856574058499</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>87.331324815750094</v>
       </c>
@@ -8309,8 +8492,17 @@
       <c r="O22">
         <v>545.26629543304398</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q22">
+        <v>88.353449106216402</v>
+      </c>
+      <c r="R22">
+        <v>0.28909618343189503</v>
+      </c>
+      <c r="S22">
+        <v>505.04830193519501</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>87.447530031204195</v>
       </c>
@@ -8347,8 +8539,17 @@
       <c r="O23">
         <v>544.52358675002995</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q23">
+        <v>89.173996448516803</v>
+      </c>
+      <c r="R23">
+        <v>0.269333901143752</v>
+      </c>
+      <c r="S23">
+        <v>503.45758676528902</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>88.287049531936603</v>
       </c>
@@ -8385,8 +8586,17 @@
       <c r="O24">
         <v>546.63705778121903</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q24">
+        <v>89.399296045303302</v>
+      </c>
+      <c r="R24">
+        <v>0.26802358747653798</v>
+      </c>
+      <c r="S24">
+        <v>503.64614963531398</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>89.098107814788804</v>
       </c>
@@ -8423,8 +8633,17 @@
       <c r="O25">
         <v>546.20874142646699</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q25">
+        <v>87.777173519134493</v>
+      </c>
+      <c r="R25">
+        <v>0.31135509708749098</v>
+      </c>
+      <c r="S25">
+        <v>504.09301447868302</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>88.135272264480506</v>
       </c>
@@ -8461,8 +8680,17 @@
       <c r="O26">
         <v>547.71153569221497</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q26">
+        <v>88.237249851226807</v>
+      </c>
+      <c r="R26">
+        <v>0.294473698137734</v>
+      </c>
+      <c r="S26">
+        <v>503.687465190887</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>88.334476947784395</v>
       </c>
@@ -8499,8 +8727,17 @@
       <c r="O27">
         <v>545.36057758331299</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q27">
+        <v>88.882303237914996</v>
+      </c>
+      <c r="R27">
+        <v>0.26118712204175798</v>
+      </c>
+      <c r="S27">
+        <v>505.29672431945801</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>89.361351728439303</v>
       </c>
@@ -8537,8 +8774,17 @@
       <c r="O28">
         <v>543.04964137077297</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q28">
+        <v>85.941612720489502</v>
+      </c>
+      <c r="R28">
+        <v>0.31737491708827198</v>
+      </c>
+      <c r="S28">
+        <v>504.03100633621199</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>89.306801557540894</v>
       </c>
@@ -8575,8 +8821,17 @@
       <c r="O29">
         <v>544.50223922729401</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q29">
+        <v>87.881517410278306</v>
+      </c>
+      <c r="R29">
+        <v>0.30841567893434002</v>
+      </c>
+      <c r="S29">
+        <v>504.01990795135498</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>88.315504789352403</v>
       </c>
@@ -8613,8 +8868,17 @@
       <c r="O30">
         <v>547.74136209487904</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q30">
+        <v>87.385869026183997</v>
+      </c>
+      <c r="R30">
+        <v>0.32520304055804999</v>
+      </c>
+      <c r="S30">
+        <v>503.82376790046601</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>87.895745038986206</v>
       </c>
@@ -8651,8 +8915,17 @@
       <c r="O31">
         <v>543.99815678596497</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q31">
+        <v>88.545542955398503</v>
+      </c>
+      <c r="R31">
+        <v>0.28942292421129601</v>
+      </c>
+      <c r="S31">
+        <v>501.82972598075798</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>88.747125864028902</v>
       </c>
@@ -8689,8 +8962,17 @@
       <c r="O32">
         <v>547.98098540306</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q32">
+        <v>89.057791233062702</v>
+      </c>
+      <c r="R32">
+        <v>0.24997637207201101</v>
+      </c>
+      <c r="S32">
+        <v>502.504124641418</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>89.370834827423096</v>
       </c>
@@ -8727,8 +9009,17 @@
       <c r="O33">
         <v>544.29760575294495</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q33">
+        <v>88.201671838760305</v>
+      </c>
+      <c r="R33">
+        <v>0.29460028703839403</v>
+      </c>
+      <c r="S33">
+        <v>501.97546529769897</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>88.737636804580603</v>
       </c>
@@ -8765,8 +9056,17 @@
       <c r="O34">
         <v>544.23738980293194</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q34">
+        <v>88.813525438308702</v>
+      </c>
+      <c r="R34">
+        <v>0.251193278323396</v>
+      </c>
+      <c r="S34">
+        <v>502.832363128662</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>88.389027118682804</v>
       </c>
@@ -8803,8 +9103,17 @@
       <c r="O35">
         <v>543.86246681213299</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q35">
+        <v>88.970047235488806</v>
+      </c>
+      <c r="R35">
+        <v>0.26526913727101797</v>
+      </c>
+      <c r="S35">
+        <v>500.71220993995598</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>88.268077373504596</v>
       </c>
@@ -8841,8 +9150,17 @@
       <c r="O36">
         <v>544.77868914604096</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q36">
+        <v>89.259374141693101</v>
+      </c>
+      <c r="R36">
+        <v>0.27159849401903202</v>
+      </c>
+      <c r="S36">
+        <v>502.38794183731</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>88.8846755027771</v>
       </c>
@@ -8879,8 +9197,17 @@
       <c r="O37">
         <v>547.13121771812405</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q37">
+        <v>89.667272567748995</v>
+      </c>
+      <c r="R37">
+        <v>0.25650285274602402</v>
+      </c>
+      <c r="S37">
+        <v>501.87644219398499</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>87.741601467132497</v>
       </c>
@@ -8917,8 +9244,17 @@
       <c r="O38">
         <v>547.16282296180702</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q38">
+        <v>88.818269968032794</v>
+      </c>
+      <c r="R38">
+        <v>0.26652290204589202</v>
+      </c>
+      <c r="S38">
+        <v>501.35289955139098</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>89.309173822402897</v>
       </c>
@@ -8955,8 +9291,17 @@
       <c r="O39">
         <v>549.94790124893098</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q39">
+        <v>89.157396554946899</v>
+      </c>
+      <c r="R39">
+        <v>0.244437376629909</v>
+      </c>
+      <c r="S39">
+        <v>502.79593753814697</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>87.722629308700505</v>
       </c>
@@ -8993,8 +9338,17 @@
       <c r="O40">
         <v>545.10195541381802</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q40">
+        <v>89.036452770233097</v>
+      </c>
+      <c r="R40">
+        <v>0.254452926719276</v>
+      </c>
+      <c r="S40">
+        <v>504.56968164443902</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>88.891786336898804</v>
       </c>
@@ -9031,8 +9385,17 @@
       <c r="O41">
         <v>547.15556144714299</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q41">
+        <v>88.327366113662706</v>
+      </c>
+      <c r="R41">
+        <v>0.28876673847038897</v>
+      </c>
+      <c r="S41">
+        <v>502.76340556144697</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>88.922619819641099</v>
       </c>
@@ -9069,8 +9432,17 @@
       <c r="O42">
         <v>552.29076719284001</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q42">
+        <v>87.639623880386296</v>
+      </c>
+      <c r="R42">
+        <v>0.30783324543025598</v>
+      </c>
+      <c r="S42">
+        <v>507.10781574249199</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>88.509970903396606</v>
       </c>
@@ -9107,8 +9479,17 @@
       <c r="O43">
         <v>547.493482589721</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q43">
+        <v>88.858586549758897</v>
+      </c>
+      <c r="R43">
+        <v>0.274864964552544</v>
+      </c>
+      <c r="S43">
+        <v>503.01429700851401</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>89.057791233062702</v>
       </c>
@@ -9145,8 +9526,17 @@
       <c r="O44">
         <v>546.67198348045304</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q44">
+        <v>88.467282056808401</v>
+      </c>
+      <c r="R44">
+        <v>0.27505873285733401</v>
+      </c>
+      <c r="S44">
+        <v>505.76502108573902</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>82.941639423370304</v>
       </c>
@@ -9183,8 +9573,17 @@
       <c r="O45">
         <v>542.47305011749199</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q45">
+        <v>88.830125331878605</v>
+      </c>
+      <c r="R45">
+        <v>0.25426941915770801</v>
+      </c>
+      <c r="S45">
+        <v>506.609098911285</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>89.072024822235093</v>
       </c>
@@ -9221,8 +9620,17 @@
       <c r="O46">
         <v>547.44016408920197</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q46">
+        <v>89.211940765380803</v>
+      </c>
+      <c r="R46">
+        <v>0.26151681250084002</v>
+      </c>
+      <c r="S46">
+        <v>504.03819203376702</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>88.782697916030799</v>
       </c>
@@ -9259,8 +9667,17 @@
       <c r="O47">
         <v>544.81893038749695</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q47">
+        <v>88.732898235321002</v>
+      </c>
+      <c r="R47">
+        <v>0.28200692942259398</v>
+      </c>
+      <c r="S47">
+        <v>501.86926364898602</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>88.906013965606604</v>
       </c>
@@ -9297,8 +9714,17 @@
       <c r="O48">
         <v>546.60061383247296</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q48">
+        <v>89.209568500518799</v>
+      </c>
+      <c r="R48">
+        <v>0.25169849239608999</v>
+      </c>
+      <c r="S48">
+        <v>504.42156839370699</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>88.336849212646399</v>
       </c>
@@ -9335,8 +9761,17 @@
       <c r="O49">
         <v>546.98892784118596</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q49">
+        <v>88.977164030075002</v>
+      </c>
+      <c r="R49">
+        <v>0.267249805656951</v>
+      </c>
+      <c r="S49">
+        <v>503.68649840354902</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>88.206416368484497</v>
       </c>
@@ -9373,8 +9808,17 @@
       <c r="O50">
         <v>543.56502509117104</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q50">
+        <v>87.786656618118201</v>
+      </c>
+      <c r="R50">
+        <v>0.28814849022857197</v>
+      </c>
+      <c r="S50">
+        <v>504.78978967666598</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>88.097327947616506</v>
       </c>
@@ -9410,6 +9854,15 @@
       </c>
       <c r="O51">
         <v>546.291284561157</v>
+      </c>
+      <c r="Q51">
+        <v>88.616693019866901</v>
+      </c>
+      <c r="R51">
+        <v>0.26249624012110501</v>
+      </c>
+      <c r="S51">
+        <v>505.93578052520701</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 200 Packet run MW 1D
</commit_message>
<xml_diff>
--- a/50TrialsVaryPackets.xlsx
+++ b/50TrialsVaryPackets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\AP-Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D732A543-9884-4BEE-8E33-F2B4A1784D14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75CAB177-267D-4F72-A91B-8D2040F6CEE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="20">
   <si>
     <t>Acc</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>CNN 2D All</t>
+  </si>
+  <si>
+    <t>v c</t>
   </si>
 </sst>
 </file>
@@ -8516,15 +8519,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:X56"/>
+  <dimension ref="A1:AB56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="L37" sqref="L37"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
@@ -8543,8 +8546,11 @@
       <c r="W1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="2:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AA1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="2:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -8599,8 +8605,17 @@
       <c r="X2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>89.899682998657198</v>
       </c>
@@ -8655,8 +8670,17 @@
       <c r="X3">
         <v>483.47402858734102</v>
       </c>
-    </row>
-    <row r="4" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z3">
+        <v>88.647520542144704</v>
+      </c>
+      <c r="AA3">
+        <v>0.29172533327497502</v>
+      </c>
+      <c r="AB3">
+        <v>471.59354948997498</v>
+      </c>
+    </row>
+    <row r="4" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>89.669644832610999</v>
       </c>
@@ -8711,8 +8735,17 @@
       <c r="X4">
         <v>475.05851984024002</v>
       </c>
-    </row>
-    <row r="5" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z4">
+        <v>89.394551515579195</v>
+      </c>
+      <c r="AA4">
+        <v>0.25142665083347998</v>
+      </c>
+      <c r="AB4">
+        <v>461.119449615478</v>
+      </c>
+    </row>
+    <row r="5" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>87.739229202270494</v>
       </c>
@@ -8767,8 +8800,17 @@
       <c r="X5">
         <v>475.72938919067298</v>
       </c>
-    </row>
-    <row r="6" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z5">
+        <v>89.271229505538898</v>
+      </c>
+      <c r="AA5">
+        <v>0.26566754305444901</v>
+      </c>
+      <c r="AB5">
+        <v>461.11307930946299</v>
+      </c>
+    </row>
+    <row r="6" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>87.928950786590505</v>
       </c>
@@ -8823,8 +8865,17 @@
       <c r="X6">
         <v>474.949491262435</v>
       </c>
-    </row>
-    <row r="7" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z6">
+        <v>89.688616991043006</v>
+      </c>
+      <c r="AA6">
+        <v>0.25564228762697799</v>
+      </c>
+      <c r="AB6">
+        <v>461.56454730033801</v>
+      </c>
+    </row>
+    <row r="7" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>87.656223773956299</v>
       </c>
@@ -8879,8 +8930,17 @@
       <c r="X7">
         <v>475.75396847724897</v>
       </c>
-    </row>
-    <row r="8" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z7">
+        <v>88.019067049026404</v>
+      </c>
+      <c r="AA7">
+        <v>0.29991020372850602</v>
+      </c>
+      <c r="AB7">
+        <v>461.12673068046502</v>
+      </c>
+    </row>
+    <row r="8" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>89.000874757766695</v>
       </c>
@@ -8935,8 +8995,17 @@
       <c r="X8">
         <v>473.405846834182</v>
       </c>
-    </row>
-    <row r="9" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z8">
+        <v>89.000874757766695</v>
+      </c>
+      <c r="AA8">
+        <v>0.28511941850529499</v>
+      </c>
+      <c r="AB8">
+        <v>465.46656298637299</v>
+      </c>
+    </row>
+    <row r="9" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>89.169257879257202</v>
       </c>
@@ -8991,8 +9060,17 @@
       <c r="X9">
         <v>475.68893241882301</v>
       </c>
-    </row>
-    <row r="10" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z9">
+        <v>88.730525970458899</v>
+      </c>
+      <c r="AA9">
+        <v>0.27735378177696901</v>
+      </c>
+      <c r="AB9">
+        <v>460.39963817596401</v>
+      </c>
+    </row>
+    <row r="10" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>89.216685295104895</v>
       </c>
@@ -9047,8 +9125,17 @@
       <c r="X10">
         <v>475.92329239845202</v>
       </c>
-    </row>
-    <row r="11" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z10">
+        <v>89.247518777847205</v>
+      </c>
+      <c r="AA10">
+        <v>0.25306278556266498</v>
+      </c>
+      <c r="AB10">
+        <v>464.23108601570101</v>
+      </c>
+    </row>
+    <row r="11" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>89.356607198715196</v>
       </c>
@@ -9103,8 +9190,17 @@
       <c r="X11">
         <v>474.27302718162503</v>
       </c>
-    </row>
-    <row r="12" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z11">
+        <v>89.079135656356797</v>
+      </c>
+      <c r="AA11">
+        <v>0.24944038304830901</v>
+      </c>
+      <c r="AB11">
+        <v>462.913558006286</v>
+      </c>
+    </row>
+    <row r="12" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>88.744753599166799</v>
       </c>
@@ -9159,8 +9255,17 @@
       <c r="X12">
         <v>474.56031656265202</v>
       </c>
-    </row>
-    <row r="13" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z12">
+        <v>85.476791858673096</v>
+      </c>
+      <c r="AA12">
+        <v>0.32642584738585301</v>
+      </c>
+      <c r="AB12">
+        <v>463.599218606948</v>
+      </c>
+    </row>
+    <row r="13" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>88.946330547332707</v>
       </c>
@@ -9215,8 +9320,17 @@
       <c r="X13">
         <v>474.399509191513</v>
       </c>
-    </row>
-    <row r="14" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z13">
+        <v>88.699692487716604</v>
+      </c>
+      <c r="AA13">
+        <v>0.27395483164948198</v>
+      </c>
+      <c r="AB13">
+        <v>462.34886145591702</v>
+      </c>
+    </row>
+    <row r="14" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>88.317877054214406</v>
       </c>
@@ -9271,8 +9385,17 @@
       <c r="X14">
         <v>475.571006774902</v>
       </c>
-    </row>
-    <row r="15" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z14">
+        <v>89.1194522380828</v>
+      </c>
+      <c r="AA14">
+        <v>0.27031771345587702</v>
+      </c>
+      <c r="AB14">
+        <v>463.07760882377602</v>
+      </c>
+    </row>
+    <row r="15" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>89.446723461151095</v>
       </c>
@@ -9327,8 +9450,17 @@
       <c r="X15">
         <v>476.75548529624899</v>
       </c>
-    </row>
-    <row r="16" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z15">
+        <v>89.847511053085299</v>
+      </c>
+      <c r="AA15">
+        <v>0.25591995566252901</v>
+      </c>
+      <c r="AB15">
+        <v>460.390878915786</v>
+      </c>
+    </row>
+    <row r="16" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>88.227760791778493</v>
       </c>
@@ -9383,8 +9515,17 @@
       <c r="X16">
         <v>475.862070322036</v>
       </c>
-    </row>
-    <row r="17" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z16">
+        <v>88.301277160644503</v>
+      </c>
+      <c r="AA16">
+        <v>0.26133078872799798</v>
+      </c>
+      <c r="AB16">
+        <v>462.88062715530299</v>
+      </c>
+    </row>
+    <row r="17" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>89.000874757766695</v>
       </c>
@@ -9439,8 +9580,17 @@
       <c r="X17">
         <v>475.50758361816401</v>
       </c>
-    </row>
-    <row r="18" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z17">
+        <v>87.457019090652395</v>
+      </c>
+      <c r="AA17">
+        <v>0.29450335650544102</v>
+      </c>
+      <c r="AB17">
+        <v>462.04888916015602</v>
+      </c>
+    </row>
+    <row r="18" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>89.211940765380803</v>
       </c>
@@ -9495,8 +9645,17 @@
       <c r="X18">
         <v>473.659565687179</v>
       </c>
-    </row>
-    <row r="19" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z18">
+        <v>88.934475183486896</v>
+      </c>
+      <c r="AA18">
+        <v>0.25481036988731598</v>
+      </c>
+      <c r="AB18">
+        <v>461.48591017722998</v>
+      </c>
+    </row>
+    <row r="19" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>88.251477479934593</v>
       </c>
@@ -9551,8 +9710,17 @@
       <c r="X19">
         <v>473.31639146804798</v>
       </c>
-    </row>
-    <row r="20" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z19">
+        <v>87.867289781570406</v>
+      </c>
+      <c r="AA19">
+        <v>0.31816218429759602</v>
+      </c>
+      <c r="AB19">
+        <v>463.88524746894802</v>
+      </c>
+    </row>
+    <row r="20" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>88.075983524322496</v>
       </c>
@@ -9607,8 +9775,17 @@
       <c r="X20">
         <v>474.595871925354</v>
       </c>
-    </row>
-    <row r="21" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z20">
+        <v>89.017480611801105</v>
+      </c>
+      <c r="AA20">
+        <v>0.257885398734092</v>
+      </c>
+      <c r="AB20">
+        <v>461.82305645942603</v>
+      </c>
+    </row>
+    <row r="21" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>88.993763923645005</v>
       </c>
@@ -9663,8 +9840,17 @@
       <c r="X21">
         <v>473.565135717391</v>
       </c>
-    </row>
-    <row r="22" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z21">
+        <v>88.799297809600802</v>
+      </c>
+      <c r="AA21">
+        <v>0.27025974393110003</v>
+      </c>
+      <c r="AB21">
+        <v>463.57051944732598</v>
+      </c>
+    </row>
+    <row r="22" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>87.331324815750094</v>
       </c>
@@ -9719,8 +9905,17 @@
       <c r="X22">
         <v>474.60574960708601</v>
       </c>
-    </row>
-    <row r="23" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z22">
+        <v>89.233285188674898</v>
+      </c>
+      <c r="AA22">
+        <v>0.25176019515860398</v>
+      </c>
+      <c r="AB22">
+        <v>462.14640021324101</v>
+      </c>
+    </row>
+    <row r="23" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>87.447530031204195</v>
       </c>
@@ -9775,8 +9970,17 @@
       <c r="X23">
         <v>477.67639923095697</v>
       </c>
-    </row>
-    <row r="24" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z23">
+        <v>89.572411775588904</v>
+      </c>
+      <c r="AA23">
+        <v>0.245837544843688</v>
+      </c>
+      <c r="AB23">
+        <v>463.55166697502102</v>
+      </c>
+    </row>
+    <row r="24" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>88.287049531936603</v>
       </c>
@@ -9831,8 +10035,17 @@
       <c r="X24">
         <v>476.15692424774102</v>
       </c>
-    </row>
-    <row r="25" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z24">
+        <v>89.010363817214895</v>
+      </c>
+      <c r="AA24">
+        <v>0.27472634441592397</v>
+      </c>
+      <c r="AB24">
+        <v>459.59633493423399</v>
+      </c>
+    </row>
+    <row r="25" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>89.098107814788804</v>
       </c>
@@ -9887,8 +10100,17 @@
       <c r="X25">
         <v>475.56362199783302</v>
       </c>
-    </row>
-    <row r="26" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z25">
+        <v>89.247518777847205</v>
+      </c>
+      <c r="AA25">
+        <v>0.26139393250298198</v>
+      </c>
+      <c r="AB25">
+        <v>461.20588707923798</v>
+      </c>
+    </row>
+    <row r="26" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>88.135272264480506</v>
       </c>
@@ -9943,8 +10165,17 @@
       <c r="X26">
         <v>476.65149116516102</v>
       </c>
-    </row>
-    <row r="27" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z26">
+        <v>88.718664646148596</v>
+      </c>
+      <c r="AA26">
+        <v>0.27351009722826503</v>
+      </c>
+      <c r="AB26">
+        <v>465.39883661270102</v>
+      </c>
+    </row>
+    <row r="27" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>88.334476947784395</v>
       </c>
@@ -9999,8 +10230,17 @@
       <c r="X27">
         <v>474.98331236839198</v>
       </c>
-    </row>
-    <row r="28" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z27">
+        <v>89.114707708358694</v>
+      </c>
+      <c r="AA27">
+        <v>0.25417985736045901</v>
+      </c>
+      <c r="AB27">
+        <v>462.37801456451399</v>
+      </c>
+    </row>
+    <row r="28" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>89.361351728439303</v>
       </c>
@@ -10055,8 +10295,17 @@
       <c r="X28">
         <v>475.80445694923401</v>
       </c>
-    </row>
-    <row r="29" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z28">
+        <v>88.694953918457003</v>
+      </c>
+      <c r="AA28">
+        <v>0.293079361334737</v>
+      </c>
+      <c r="AB28">
+        <v>463.96956706047001</v>
+      </c>
+    </row>
+    <row r="29" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>89.306801557540894</v>
       </c>
@@ -10111,8 +10360,17 @@
       <c r="X29">
         <v>474.51709723472499</v>
       </c>
-    </row>
-    <row r="30" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z29">
+        <v>89.143168926238999</v>
+      </c>
+      <c r="AA29">
+        <v>0.24245275793190299</v>
+      </c>
+      <c r="AB29">
+        <v>459.76927876472399</v>
+      </c>
+    </row>
+    <row r="30" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>88.315504789352403</v>
       </c>
@@ -10167,8 +10425,17 @@
       <c r="X30">
         <v>475.62811589240999</v>
       </c>
-    </row>
-    <row r="31" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z30">
+        <v>89.000874757766695</v>
+      </c>
+      <c r="AA30">
+        <v>0.25922572803289601</v>
+      </c>
+      <c r="AB30">
+        <v>460.57213950157097</v>
+      </c>
+    </row>
+    <row r="31" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>87.895745038986206</v>
       </c>
@@ -10223,8 +10490,17 @@
       <c r="X31">
         <v>473.84651637077297</v>
       </c>
-    </row>
-    <row r="32" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z31">
+        <v>88.481515645980807</v>
+      </c>
+      <c r="AA31">
+        <v>0.29369116100866999</v>
+      </c>
+      <c r="AB31">
+        <v>462.12938785552899</v>
+      </c>
+    </row>
+    <row r="32" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>88.747125864028902</v>
       </c>
@@ -10279,8 +10555,17 @@
       <c r="X32">
         <v>473.736820936203</v>
       </c>
-    </row>
-    <row r="33" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z32">
+        <v>89.181113243102999</v>
+      </c>
+      <c r="AA32">
+        <v>0.25030409383191898</v>
+      </c>
+      <c r="AB32">
+        <v>462.83479976654002</v>
+      </c>
+    </row>
+    <row r="33" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>89.370834827423096</v>
       </c>
@@ -10335,8 +10620,17 @@
       <c r="X33">
         <v>476.33879399299599</v>
       </c>
-    </row>
-    <row r="34" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z33">
+        <v>87.864917516708303</v>
+      </c>
+      <c r="AA33">
+        <v>0.298987714733779</v>
+      </c>
+      <c r="AB33">
+        <v>462.400925159454</v>
+      </c>
+    </row>
+    <row r="34" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>88.737636804580603</v>
       </c>
@@ -10391,8 +10685,17 @@
       <c r="X34">
         <v>475.83533501624999</v>
       </c>
-    </row>
-    <row r="35" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z34">
+        <v>88.777953386306706</v>
+      </c>
+      <c r="AA34">
+        <v>0.27118690311007498</v>
+      </c>
+      <c r="AB34">
+        <v>464.17543506622297</v>
+      </c>
+    </row>
+    <row r="35" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>88.389027118682804</v>
       </c>
@@ -10447,8 +10750,17 @@
       <c r="X35">
         <v>474.96280455589198</v>
       </c>
-    </row>
-    <row r="36" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z35">
+        <v>88.815897703170705</v>
+      </c>
+      <c r="AA35">
+        <v>0.27288601945761498</v>
+      </c>
+      <c r="AB35">
+        <v>462.15470814704798</v>
+      </c>
+    </row>
+    <row r="36" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>88.268077373504596</v>
       </c>
@@ -10503,8 +10815,17 @@
       <c r="X36">
         <v>472.89153981208801</v>
       </c>
-    </row>
-    <row r="37" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z36">
+        <v>89.306801557540894</v>
+      </c>
+      <c r="AA36">
+        <v>0.24464437900555899</v>
+      </c>
+      <c r="AB36">
+        <v>460.146674156188</v>
+      </c>
+    </row>
+    <row r="37" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>88.8846755027771</v>
       </c>
@@ -10559,8 +10880,17 @@
       <c r="X37">
         <v>475.616893529891</v>
       </c>
-    </row>
-    <row r="38" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z37">
+        <v>89.169257879257202</v>
+      </c>
+      <c r="AA37">
+        <v>0.25969924925655202</v>
+      </c>
+      <c r="AB37">
+        <v>461.79513716697602</v>
+      </c>
+    </row>
+    <row r="38" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>87.741601467132497</v>
       </c>
@@ -10615,8 +10945,17 @@
       <c r="X38">
         <v>476.06138896942099</v>
       </c>
-    </row>
-    <row r="39" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z38">
+        <v>87.978750467300401</v>
+      </c>
+      <c r="AA38">
+        <v>0.31268606102309399</v>
+      </c>
+      <c r="AB38">
+        <v>461.53372931480402</v>
+      </c>
+    </row>
+    <row r="39" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>89.309173822402897</v>
       </c>
@@ -10671,8 +11010,17 @@
       <c r="X39">
         <v>474.98520922660799</v>
       </c>
-    </row>
-    <row r="40" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z39">
+        <v>89.323407411575303</v>
+      </c>
+      <c r="AA39">
+        <v>0.25088632003663403</v>
+      </c>
+      <c r="AB39">
+        <v>462.360209465026</v>
+      </c>
+    </row>
+    <row r="40" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>87.722629308700505</v>
       </c>
@@ -10700,6 +11048,9 @@
       <c r="L40">
         <v>566.00424218177795</v>
       </c>
+      <c r="M40" t="s">
+        <v>19</v>
+      </c>
       <c r="N40">
         <v>88.426971435546804</v>
       </c>
@@ -10727,8 +11078,17 @@
       <c r="X40">
         <v>473.39102768897999</v>
       </c>
-    </row>
-    <row r="41" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z40">
+        <v>87.532907724380493</v>
+      </c>
+      <c r="AA40">
+        <v>0.338108114561606</v>
+      </c>
+      <c r="AB40">
+        <v>460.29124689102099</v>
+      </c>
+    </row>
+    <row r="41" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>88.891786336898804</v>
       </c>
@@ -10783,8 +11143,17 @@
       <c r="X41">
         <v>475.56896162033001</v>
       </c>
-    </row>
-    <row r="42" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z41">
+        <v>88.996136188506995</v>
+      </c>
+      <c r="AA41">
+        <v>0.26961057123740201</v>
+      </c>
+      <c r="AB41">
+        <v>463.76413369178698</v>
+      </c>
+    </row>
+    <row r="42" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>88.922619819641099</v>
       </c>
@@ -10839,8 +11208,17 @@
       <c r="X42">
         <v>475.40050315856899</v>
       </c>
-    </row>
-    <row r="43" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z42">
+        <v>89.529728889465304</v>
+      </c>
+      <c r="AA42">
+        <v>0.24368283545649699</v>
+      </c>
+      <c r="AB42">
+        <v>463.56668210029602</v>
+      </c>
+    </row>
+    <row r="43" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>88.509970903396606</v>
       </c>
@@ -10895,8 +11273,17 @@
       <c r="X43">
         <v>475.44683098793001</v>
       </c>
-    </row>
-    <row r="44" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z43">
+        <v>88.839614391326904</v>
+      </c>
+      <c r="AA43">
+        <v>0.25797176401899802</v>
+      </c>
+      <c r="AB43">
+        <v>462.25898408889702</v>
+      </c>
+    </row>
+    <row r="44" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>89.057791233062702</v>
       </c>
@@ -10951,8 +11338,17 @@
       <c r="X44">
         <v>475.22317361831603</v>
       </c>
-    </row>
-    <row r="45" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z44">
+        <v>89.188230037689195</v>
+      </c>
+      <c r="AA44">
+        <v>0.26381842122476601</v>
+      </c>
+      <c r="AB44">
+        <v>460.543656826019</v>
+      </c>
+    </row>
+    <row r="45" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B45" s="4">
         <v>82.941639423370304</v>
       </c>
@@ -11007,8 +11403,17 @@
       <c r="X45">
         <v>473.21894955635003</v>
       </c>
-    </row>
-    <row r="46" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z45">
+        <v>89.188230037689195</v>
+      </c>
+      <c r="AA45">
+        <v>0.25237014731330198</v>
+      </c>
+      <c r="AB45">
+        <v>463.21752071380598</v>
+      </c>
+    </row>
+    <row r="46" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>89.072024822235093</v>
       </c>
@@ -11063,8 +11468,17 @@
       <c r="X46">
         <v>475.72774577140802</v>
       </c>
-    </row>
-    <row r="47" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z46">
+        <v>87.891006469726506</v>
+      </c>
+      <c r="AA46">
+        <v>0.32553704761340202</v>
+      </c>
+      <c r="AB46">
+        <v>460.541975975036</v>
+      </c>
+    </row>
+    <row r="47" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>88.782697916030799</v>
       </c>
@@ -11119,8 +11533,17 @@
       <c r="X47">
         <v>475.782336473464</v>
       </c>
-    </row>
-    <row r="48" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z47">
+        <v>88.460171222686697</v>
+      </c>
+      <c r="AA47">
+        <v>0.27916198640133699</v>
+      </c>
+      <c r="AB47">
+        <v>463.69074869155799</v>
+      </c>
+    </row>
+    <row r="48" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B48">
         <v>88.906013965606604</v>
       </c>
@@ -11175,8 +11598,17 @@
       <c r="X48">
         <v>474.92248678207397</v>
       </c>
-    </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Z48">
+        <v>88.858586549758897</v>
+      </c>
+      <c r="AA48">
+        <v>0.27800204176438498</v>
+      </c>
+      <c r="AB48">
+        <v>463.50334715843201</v>
+      </c>
+    </row>
+    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B49">
         <v>88.336849212646399</v>
       </c>
@@ -11231,8 +11663,17 @@
       <c r="X49">
         <v>475.63016104698102</v>
       </c>
-    </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Z49">
+        <v>88.455426692962604</v>
+      </c>
+      <c r="AA49">
+        <v>0.27894910599501899</v>
+      </c>
+      <c r="AB49">
+        <v>463.32916593551602</v>
+      </c>
+    </row>
+    <row r="50" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B50">
         <v>88.206416368484497</v>
       </c>
@@ -11287,8 +11728,17 @@
       <c r="X50">
         <v>474.57900500297501</v>
       </c>
-    </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Z50">
+        <v>88.000094890594397</v>
+      </c>
+      <c r="AA50">
+        <v>0.28667592244733697</v>
+      </c>
+      <c r="AB50">
+        <v>462.64667034149102</v>
+      </c>
+    </row>
+    <row r="51" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B51">
         <v>88.097327947616506</v>
       </c>
@@ -11343,8 +11793,17 @@
       <c r="X51">
         <v>475.34892082214299</v>
       </c>
-    </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Z51">
+        <v>89.043563604354802</v>
+      </c>
+      <c r="AA51">
+        <v>0.24802463422834001</v>
+      </c>
+      <c r="AB51">
+        <v>462.66078042983997</v>
+      </c>
+    </row>
+    <row r="53" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>14</v>
       </c>
@@ -11420,8 +11879,20 @@
         <f>AVERAGE(X3:X51)</f>
         <v>475.26840829362646</v>
       </c>
-    </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Z53" s="2">
+        <f>AVERAGE(Z3:Z51)</f>
+        <v>88.759563042193022</v>
+      </c>
+      <c r="AA53" s="2">
+        <f>AVERAGE(AA3:AA51)</f>
+        <v>0.27236671204458485</v>
+      </c>
+      <c r="AB53" s="2">
+        <f>AVERAGE(AB3:AB51)</f>
+        <v>462.5055727326137</v>
+      </c>
+    </row>
+    <row r="54" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>13</v>
       </c>
@@ -11497,8 +11968,20 @@
         <f>AVERAGE(X3:X15,X17:X51)</f>
         <v>475.25604033470125</v>
       </c>
-    </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Z54">
+        <f>AVERAGE(Z3:Z51)</f>
+        <v>88.759563042193022</v>
+      </c>
+      <c r="AA54">
+        <f>AVERAGE(AA3:AA51)</f>
+        <v>0.27236671204458485</v>
+      </c>
+      <c r="AB54">
+        <f>AVERAGE(AB3:AB51)</f>
+        <v>462.5055727326137</v>
+      </c>
+    </row>
+    <row r="56" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B56">
         <v>1</v>
       </c>
@@ -11516,6 +11999,9 @@
       </c>
       <c r="V56">
         <v>1</v>
+      </c>
+      <c r="Z56">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>